<commit_message>
Updated data and logs.
</commit_message>
<xml_diff>
--- a/data/raw_data/04-2024_raw_listings.xlsx
+++ b/data/raw_data/04-2024_raw_listings.xlsx
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="O2" s="2" t="n">
-        <v>45411.78623892875</v>
+        <v>45411.7917418608</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="O3" s="2" t="n">
-        <v>45411.78623892875</v>
+        <v>45411.7917418608</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="O4" s="2" t="n">
-        <v>45411.78623892875</v>
+        <v>45411.7917418608</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -831,7 +831,7 @@
         </is>
       </c>
       <c r="O5" s="2" t="n">
-        <v>45411.78623892875</v>
+        <v>45411.7917418608</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
@@ -911,7 +911,7 @@
         </is>
       </c>
       <c r="O6" s="2" t="n">
-        <v>45411.78623892875</v>
+        <v>45411.7917418608</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="O7" s="2" t="n">
-        <v>45411.78623892875</v>
+        <v>45411.7917418608</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
@@ -1071,7 +1071,7 @@
         </is>
       </c>
       <c r="O8" s="2" t="n">
-        <v>45411.78623892875</v>
+        <v>45411.7917418608</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -1151,7 +1151,7 @@
         </is>
       </c>
       <c r="O9" s="2" t="n">
-        <v>45411.78623892875</v>
+        <v>45411.7917418608</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>

</xml_diff>